<commit_message>
Adjust fuel consumption for fleet modelling
</commit_message>
<xml_diff>
--- a/rmnd_lca/data/additional_inventories/lci-synfuels-from-methanol.xlsx
+++ b/rmnd_lca/data/additional_inventories/lci-synfuels-from-methanol.xlsx
@@ -689,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H859"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A817" workbookViewId="0">
-      <selection activeCell="G835" sqref="G835"/>
+    <sheetView tabSelected="1" topLeftCell="A353" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2721,7 +2721,7 @@
         <v>11</v>
       </c>
       <c r="B148" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>